<commit_message>
check comparision between evidencemap studylist and extracted data, correct spelling in evidencemap-cleaning, find double-publications and determine data that still needs to be extracted
</commit_message>
<xml_diff>
--- a/02_data/cleandata/studies_to_check.xlsx
+++ b/02_data/cleandata/studies_to_check.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -502,106 +502,86 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CHR Population</t>
+          <t>Healthy Population</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CHR state</t>
+          <t>Psychotic-like-experiences</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Addington (2012)</t>
+          <t>van Gastel (2014)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Addington</t>
+          <t>van Gastel</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Carney (2017)</t>
+          <t>Ragazzi(2017)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>current cannabis use</t>
+          <t>cannabis use</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>CHR state</t>
+          <t>total PLE</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>1.556</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1.061</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2.28</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0.023</t>
+          <t>prospective cohort</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>705</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>unclear</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>Addington</t>
+          <t>vanGastel</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>CHR</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>addington_2012_chr</t>
+          <t>vangastel_2014_hp</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>addington_2012</t>
+          <t>vangastel_2014</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>maybe</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="Z2">
-        <v>4</v>
+        <v>314</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
@@ -610,54 +590,69 @@
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>addington_2017</t>
+          <t>valmaggia_2014</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>Healthy Population</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>Any psychosis outcome</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Albertella (2018)</t>
+          <t>Zammit (2004)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Albertella</t>
+          <t>Zammit</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2004</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Polkosnik(2021)</t>
+          <t>Moore (2007)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Low cannabis use</t>
+          <t>most frequent use</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>Any psychosis outcome</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>prospective cohort</t>
+          <t>longitudinal</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>3.1</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>1.72</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>5.58</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -667,31 +662,31 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>Albertella</t>
+          <t>Zammit</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>EnvMod</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>albertella_2018_envmod</t>
+          <t>zammit_2004_hp</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>albertella_2018</t>
+          <t>zammit_2004</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>maybe</t>
         </is>
       </c>
       <c r="Z3">
-        <v>8</v>
+        <v>334</v>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
@@ -700,98 +695,108 @@
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>berger_2016</t>
+          <t>zammit_2002</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>Healthy Population</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>Any psychosis outcome</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bechtold (2015)</t>
+          <t>GAP data (2012)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Bechtold</t>
+          <t>GAP data</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Hosseini(2019)</t>
+          <t>Moore (2007)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Age of first use</t>
+          <t>most frequent  use</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>Any psychosis outcome</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>506</t>
+          <t>prospective cohort</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>in tabelle (supplementary material, Appendix 3)</t>
+          <t>4.38</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>ES?</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>5.81</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>Bechtold</t>
+          <t>GAPdata</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>EnvMod</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>bechtold_2015_envmod</t>
+          <t>gapdata_2012_hp</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>bechtold_2015</t>
+          <t>gapdata_2012</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>maybe</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="Z4">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
@@ -800,39 +805,39 @@
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>bechtold_2016</t>
+          <t>vandijk_2012</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>Healthy Population</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>Any psychosis outcome</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bhattacharrya (2020)</t>
+          <t>Caspi (2005)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Bhattacharrya</t>
+          <t>Caspi</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Athanassiou (2021)</t>
+          <t>Sorkhou(2021)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -842,7 +847,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>Any psychosis outcome</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -850,34 +855,39 @@
           <t>longitudinal</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>803</t>
+        </is>
+      </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>3.44</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>OR</t>
+          <t>not reported</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>Bhattacharrya</t>
+          <t>Caspi</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>bhattacharrya_2020_p</t>
+          <t>caspi_2005_hp</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>bhattacharrya_2020</t>
+          <t>caspi_2005</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -886,7 +896,7 @@
         </is>
       </c>
       <c r="Z5">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
@@ -895,39 +905,39 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>harley_2010</t>
+          <t>isaac_2005</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CHR Population</t>
+          <t>Healthy Population</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>transition</t>
+          <t>Any psychosis outcome</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bloeman (2010)</t>
+          <t>Griffith-Lendering (2013)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Bloeman</t>
+          <t>Griffith-Lendering</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Oliver(2020)</t>
+          <t>Sorkhou(2021)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -937,32 +947,47 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>transition to psychosis</t>
+          <t>Any psychosis outcome</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>cohort</t>
+          <t>longitudinal</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2120</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>not reported</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>Bloeman</t>
+          <t>Griffith-Lendering</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>CHR</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>bloeman_2010_chr</t>
+          <t>griffith-lendering_2013_hp</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>bloeman_2010</t>
+          <t>griffith-lendering_2013</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -971,7 +996,7 @@
         </is>
       </c>
       <c r="Z6">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
@@ -980,39 +1005,39 @@
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>bloemen_2009</t>
+          <t>kristensen_2007</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Healthy Population</t>
+          <t>CHR Population</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Any psychosis outcome</t>
+          <t>transition</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Caspi (2005)</t>
+          <t>Dragt  (2011)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Caspi</t>
+          <t>Dragt</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sorkhou(2021)</t>
+          <t>van der Meer (2012)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1022,47 +1047,37 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Any psychosis outcome</t>
+          <t>transition to psychosis</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>longitudinal</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>803</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>not reported</t>
+          <t>cohort</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>Caspi</t>
+          <t>Dragt</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>CHR</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>caspi_2005_hp</t>
+          <t>dragt_2011_chr</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>caspi_2005</t>
+          <t>dragt_2011</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -1071,7 +1086,7 @@
         </is>
       </c>
       <c r="Z7">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
@@ -1080,29 +1095,29 @@
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>isaac_2005</t>
+          <t>dragt_2010</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>CHR Population</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>symptoms</t>
+          <t>transition</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Degenhardt (2007)</t>
+          <t>Kristensen and Cadenhead (2007)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Degenhardt</t>
+          <t>Kristensen and Cadenhead</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1112,7 +1127,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Zammit (2008)</t>
+          <t>van der Meer (2012)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1122,32 +1137,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>positive symptoms</t>
+          <t>transition to psychosis</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>longitudinal</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>0.13</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>0.26</t>
+          <t>cohort</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1157,22 +1152,22 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>Degenhardt</t>
+          <t>KristensenandCadenhead</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CHR</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>degenhardt_2007_p</t>
+          <t>kristensenandcadenhead_2007_chr</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>degenhardt_2007</t>
+          <t>kristensenandcadenhead_2007</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -1181,7 +1176,7 @@
         </is>
       </c>
       <c r="Z8">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
@@ -1190,7 +1185,7 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>degenhardt_2001</t>
+          <t>kristensen_2007</t>
         </is>
       </c>
     </row>
@@ -1207,17 +1202,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Deighton (2016)</t>
+          <t>Bloeman (2010)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Deighton</t>
+          <t>Bloemen</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1242,7 +1237,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>Deighton</t>
+          <t>Bloemen</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
@@ -1252,12 +1247,12 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>deighton_2016_chr</t>
+          <t>bloemen_2010_chr</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>deighton_2016</t>
+          <t>bloemen_2010</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1266,7 +1261,7 @@
         </is>
       </c>
       <c r="Z9">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
@@ -1275,49 +1270,49 @@
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>bechtold_2016</t>
+          <t>bloemen_2009</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>CHR Population</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>transition</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Di Forti (2014)</t>
+          <t>Deighton (2016)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Di Forti</t>
+          <t>Deighton</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Hosseini(2019)</t>
+          <t>Oliver(2020)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Age of first use</t>
+          <t>cannabis use</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>transition to psychosis</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1325,39 +1320,24 @@
           <t>cohort</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>410</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>in tabelle (supplementary material, Appendix 3)</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>DiForti</t>
+          <t>Deighton</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>EnvMod</t>
+          <t>CHR</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>diforti_2014_envmod</t>
+          <t>deighton_2016_chr</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>diforti_2014</t>
+          <t>deighton_2016</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -1366,7 +1346,7 @@
         </is>
       </c>
       <c r="Z10">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
@@ -1375,7 +1355,7 @@
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>diforti_2009</t>
+          <t>bechtold_2016</t>
         </is>
       </c>
     </row>
@@ -1392,17 +1372,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dragt (2011)</t>
+          <t>Lavoie (2014)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Dragt</t>
+          <t>Lavoie</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1427,7 +1407,7 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>Dragt</t>
+          <t>Lavoie</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
@@ -1437,12 +1417,12 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>dragt_2011_chr</t>
+          <t>lavoie_2014_chr</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>dragt_2011</t>
+          <t>lavoie_2014</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -1451,7 +1431,7 @@
         </is>
       </c>
       <c r="Z11">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
@@ -1460,39 +1440,39 @@
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>dragt_2010</t>
+          <t>lavoie_2012</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>CHR Population</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>CHR symptoms</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Emsley (2019)</t>
+          <t>Peters  (2009)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Emsley</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2009</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Athanassiou (2021)</t>
+          <t>Van de Meer(2012)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1502,42 +1482,37 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>CHR symptoms</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>longitudinal</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>4.5</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>OR</t>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>Emsley</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CHR</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>emsley_2019_p</t>
+          <t>peters_2009_chr</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>emsley_2019</t>
+          <t>peters_2009</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -1546,7 +1521,7 @@
         </is>
       </c>
       <c r="Z12">
-        <v>96</v>
+        <v>232</v>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
@@ -1555,108 +1530,113 @@
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>emsley_2020</t>
+          <t>patel_2019</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Healthy Population</t>
+          <t>CHR Population</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Any psychosis outcome</t>
+          <t>CHR symptoms</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GAP data (2012)</t>
+          <t>Van Tricht (2013)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>GAP data</t>
+          <t>Van Tricht</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Moore (2007)</t>
+          <t>Carney (2017)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>most frequent  use</t>
+          <t>cannabis use</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Any psychosis outcome</t>
+          <t>Positive Symptoms</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>prospective cohort</t>
+          <t>cohort</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>4.38</t>
+          <t>7.2999999999999995E-2</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>ES?</t>
+          <t>Hedges g</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>-0.536</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>5.81</t>
+          <t>0.681</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>0.815</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>GAPdata</t>
+          <t>VanTricht</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>CHR</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>gapdata_2012_hp</t>
+          <t>vantricht_2013_chr</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>gapdata_2012</t>
+          <t>vantricht_2013</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>maybe</t>
         </is>
       </c>
       <c r="Z13">
-        <v>118</v>
+        <v>317</v>
       </c>
       <c r="AA13" t="inlineStr">
         <is>
@@ -1665,89 +1645,79 @@
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>vandijk_2012</t>
+          <t>vantricht_2014</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Healthy Population</t>
+          <t>CHR Population</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Any psychosis outcome</t>
+          <t>CHR symptoms</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Griffith-Lendering (2013)</t>
+          <t>Winton-Brown (2014)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Griffith-Lendering</t>
+          <t>Winton-Brown</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Sorkhou(2021)</t>
+          <t>Farris (2019)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>cannabis use</t>
+          <t>Cannabis use</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Any psychosis outcome</t>
+          <t>Negative Symptoms</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>longitudinal</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>2120</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>not reported</t>
+          <t>cohort</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>Griffith-Lendering</t>
+          <t>Winton-Brown</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>CHR</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>griffith-lendering_2013_hp</t>
+          <t>winton-brown_2014_chr</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>griffith-lendering_2013</t>
+          <t>winton-brown_2014</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
@@ -1756,7 +1726,7 @@
         </is>
       </c>
       <c r="Z14">
-        <v>129</v>
+        <v>331</v>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
@@ -1765,84 +1735,104 @@
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>kristensen_2007</t>
+          <t>mustonen_2018</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>CHR Population</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>CHR state</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Hadden (2016)</t>
+          <t>Addington (2012)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Hadden</t>
+          <t>Addington</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Athanassiou (2021)</t>
+          <t>Carney (2017)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>cannabis use</t>
+          <t>current cannabis use</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>CHR state</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>longitudinal</t>
+          <t>cohort</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>-0.1</t>
+          <t>1.556</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>B estimate</t>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>1.061</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>2.28</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>0.023</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>Hadden</t>
+          <t>Addington</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CHR</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>hadden_2016_p</t>
+          <t>addington_2012_chr</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>hadden_2016</t>
+          <t>addington_2012</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -1851,7 +1841,7 @@
         </is>
       </c>
       <c r="Z15">
-        <v>133</v>
+        <v>4</v>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
@@ -1860,64 +1850,74 @@
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>hadden_2026</t>
+          <t>addington_2017</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>Psychosis Population</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>symptoms</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Henquet (2004)</t>
+          <t>Degenhardt (2007)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Henquet</t>
+          <t>Degenhardt</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Hosseini(2019)</t>
+          <t>Zammit (2008)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Age of first use</t>
+          <t>cannabis use</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>any psychosis outcome</t>
+          <t>positive symptoms</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>2437</t>
+          <t>longitudinal</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>in tabelle (supplementary material, Appendix 3)</t>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>0.26</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1927,22 +1927,22 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>Henquet</t>
+          <t>Degenhardt</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>EnvMod</t>
+          <t>P</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>henquet_2004_envmod</t>
+          <t>degenhardt_2007_p</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>henquet_2004</t>
+          <t>degenhardt_2007</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
@@ -1951,7 +1951,7 @@
         </is>
       </c>
       <c r="Z16">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
@@ -1960,39 +1960,39 @@
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>henquet_2005</t>
+          <t>degenhardt_2001</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CHR Population</t>
+          <t>Psychosis Population</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>transition</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Kristensen and Cadenhead (2007)</t>
+          <t>Hadden (2016)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Kristensen and Cadenhead</t>
+          <t>Hadden</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>van der Meer (2012)</t>
+          <t>Athanassiou (2021)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2002,37 +2002,42 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>transition to psychosis</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>Yes</t>
+          <t>longitudinal</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>-0.1</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>B estimate</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>KristensenandCadenhead</t>
+          <t>Hadden</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>CHR</t>
+          <t>P</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>kristensenandcadenhead_2007_chr</t>
+          <t>hadden_2016_p</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>kristensenandcadenhead_2007</t>
+          <t>hadden_2018</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -2041,7 +2046,7 @@
         </is>
       </c>
       <c r="Z17">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
@@ -2050,39 +2055,39 @@
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>kristensen_2007</t>
+          <t>hadden_2026</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CHR Population</t>
+          <t>Psychosis Population</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>transition</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Lavoie (2014)</t>
+          <t>Oullette-Plamondon (2017)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Lavoie</t>
+          <t>Ouellett-Plamondon</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Oliver(2020)</t>
+          <t>Athanassiou (2021)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2092,32 +2097,42 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>transition to psychosis</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>cohort</t>
+          <t>longitudinal</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Cohen's D</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>Lavoie</t>
+          <t>Ouellett-Plamondon</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>CHR</t>
+          <t>P</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>lavoie_2014_chr</t>
+          <t>ouellett-plamondon_2017_p</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>lavoie_2014</t>
+          <t>ouellett-plamondon_2017</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -2126,7 +2141,7 @@
         </is>
       </c>
       <c r="Z18">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="AA18" t="inlineStr">
         <is>
@@ -2135,44 +2150,44 @@
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>lavoie_2012</t>
+          <t>ouellet-plamondon_2017</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>Psychosis Population</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Environmental Moderators</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Marwaha (2018)</t>
+          <t>Seddon (2016)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Marwaha</t>
+          <t>Seddon</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Godin(2022)</t>
+          <t>Athanassiou (2021)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>High cannabis use</t>
+          <t>cannabis use</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -2185,29 +2200,34 @@
           <t>longitudinal</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>Yes</t>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2.14</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>B estimate</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>Marwaha</t>
+          <t>Seddon</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>EnvMod</t>
+          <t>P</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>marwaha_2018_envmod</t>
+          <t>seddon_2016_p</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>marwaha_2018</t>
+          <t>seddon_2016</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -2216,7 +2236,7 @@
         </is>
       </c>
       <c r="Z19">
-        <v>195</v>
+        <v>277</v>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
@@ -2225,7 +2245,7 @@
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>mizrahi_2014</t>
+          <t>seddon_2015</t>
         </is>
       </c>
     </row>
@@ -2242,17 +2262,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Oullette-Plamondon (2017)</t>
+          <t>Bhattacharrya (2020)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Oullett-Plamondon</t>
+          <t>Bhattacharrya</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2277,17 +2297,17 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>3.44</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Cohen's D</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>Oullett-Plamondon</t>
+          <t>Bhattacharrya</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
@@ -2297,12 +2317,12 @@
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>oullett-plamondon_2017_p</t>
+          <t>bhattacharrya_2020_p</t>
         </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>oullett-plamondon_2017</t>
+          <t>bhattacharrya_2020</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
@@ -2311,7 +2331,7 @@
         </is>
       </c>
       <c r="Z20">
-        <v>224</v>
+        <v>38</v>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
@@ -2320,49 +2340,49 @@
       </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>ouellet-plamondon_2017</t>
+          <t>harley_2010</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CHR Population</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CHR symptoms</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Peters  (2009)</t>
+          <t>Bechtold (2015)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Bechtold</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Van de Meer(2012)</t>
+          <t>Hosseini(2019)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>cannabis use</t>
+          <t>Age of first use</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>CHR symptoms</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2370,29 +2390,39 @@
           <t>cohort</t>
         </is>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>506</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>in tabelle (supplementary material, Appendix 3)</t>
+        </is>
+      </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Bechtold</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>CHR</t>
+          <t>EnvMod</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>peters_2009_chr</t>
+          <t>bechtold_2015_envmod</t>
         </is>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>peters_2009</t>
+          <t>bechtold_2015</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2401,7 +2431,7 @@
         </is>
       </c>
       <c r="Z21">
-        <v>232</v>
+        <v>33</v>
       </c>
       <c r="AA21" t="inlineStr">
         <is>
@@ -2410,84 +2440,89 @@
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>patel_2019</t>
+          <t>bechtold_2016</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>Environmental Moderators</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Henquet (2004)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Henquet</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Hosseini(2019)</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Age of first use</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
           <t>any psychosis outcome</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Schimmelmann (2011)</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Schimmelmannn</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2011</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Athanassiou (2021)</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>cannabis use</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>any psychosis outcome</t>
-        </is>
-      </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>longitudinal</t>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>2437</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0.46</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>V</t>
+          <t>in tabelle (supplementary material, Appendix 3)</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>Schimmelmannn</t>
+          <t>Henquet</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>EnvMod</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>schimmelmannn_2011_p</t>
+          <t>henquet_2004_envmod</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>schimmelmannn_2011</t>
+          <t>henquet_2004</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -2496,7 +2531,7 @@
         </is>
       </c>
       <c r="Z22">
-        <v>270</v>
+        <v>138</v>
       </c>
       <c r="AA22" t="inlineStr">
         <is>
@@ -2505,7 +2540,7 @@
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>schimmelmann_2012</t>
+          <t>henquet_2005</t>
         </is>
       </c>
     </row>
@@ -2522,27 +2557,27 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Schimmelmann (2012)</t>
+          <t>Di Forti (2014)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Schimmelmannn</t>
+          <t>Di Forti</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Godin(2022)</t>
+          <t>Hosseini(2019)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>High cannabis use</t>
+          <t>Age of first use</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2552,7 +2587,17 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>longitudinal</t>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>410</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>in tabelle (supplementary material, Appendix 3)</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2562,7 +2607,7 @@
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>Schimmelmannn</t>
+          <t>DiForti</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
@@ -2572,12 +2617,12 @@
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>schimmelmannn_2012_envmod</t>
+          <t>diforti_2014_envmod</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>schimmelmannn_2012</t>
+          <t>diforti_2014</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -2586,7 +2631,7 @@
         </is>
       </c>
       <c r="Z23">
-        <v>271</v>
+        <v>86</v>
       </c>
       <c r="AA23" t="inlineStr">
         <is>
@@ -2595,84 +2640,79 @@
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>schimmelmann_2012</t>
+          <t>diforti_2009</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>Environmental Moderators</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Marwaha (2018)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Marwaha</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Godin(2022)</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>High cannabis use</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
           <t>any psychosis outcome</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Seddon (2016)</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Seddon</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Athanassiou (2021)</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>cannabis use</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>any psychosis outcome</t>
-        </is>
-      </c>
       <c r="I24" t="inlineStr">
         <is>
           <t>longitudinal</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>2.14</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>B estimate</t>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>Seddon</t>
+          <t>Marwaha</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>EnvMod</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>seddon_2016_p</t>
+          <t>marwaha_2018_envmod</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>seddon_2016</t>
+          <t>marwaha_2018</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -2681,7 +2721,7 @@
         </is>
       </c>
       <c r="Z24">
-        <v>279</v>
+        <v>195</v>
       </c>
       <c r="AA24" t="inlineStr">
         <is>
@@ -2690,74 +2730,54 @@
       </c>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>seddon_2015</t>
+          <t>mizrahi_2014</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>relapse</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Sorbaca (2003)</t>
+          <t>Albertella (2018)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Sorbaca</t>
+          <t>Albertella</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Schoeler (2016)</t>
+          <t>Polkosnik(2021)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>continued vs non-use</t>
+          <t>Low cannabis use</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Relapse</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>longitudinal</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>0·02</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>1·22</t>
+          <t>prospective cohort</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2767,31 +2787,31 @@
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>Sorbaca</t>
+          <t>Albertella</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>EnvMod</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
         <is>
-          <t>sorbaca_2003_p</t>
+          <t>albertella_2018_envmod</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>sorbaca_2003</t>
+          <t>albertella_2018</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>maybe</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="Z25">
-        <v>296</v>
+        <v>8</v>
       </c>
       <c r="AA25" t="inlineStr">
         <is>
@@ -2800,627 +2820,7 @@
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>sorbara_2003</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Healthy Population</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>psychotic symptoms</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Tien &amp; Anthony (1990)</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Tien &amp; Anthony</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>1990</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Semple (2005)</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>cannabis use</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Psychotic symptoms</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>prospective cohort</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>4994</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>2.65</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>Tien&amp;Anthony</t>
-        </is>
-      </c>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>HP</t>
-        </is>
-      </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>tien&amp;anthony_1990_hp</t>
-        </is>
-      </c>
-      <c r="X26" t="inlineStr">
-        <is>
-          <t>tien&amp;anthony_1990</t>
-        </is>
-      </c>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="Z26">
-        <v>309</v>
-      </c>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB26" t="inlineStr">
-        <is>
-          <t>tien_1990</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Healthy Population</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Psychotic-like-experiences</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Van Gastel (2014)</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Van Gastel</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Ragazzi(2017)</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>cannabis use</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>positive PLE</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>prospective cohort</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>705</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>VanGastel</t>
-        </is>
-      </c>
-      <c r="V27" t="inlineStr">
-        <is>
-          <t>HP</t>
-        </is>
-      </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>vangastel_2014_hp</t>
-        </is>
-      </c>
-      <c r="X27" t="inlineStr">
-        <is>
-          <t>vangastel_2014</t>
-        </is>
-      </c>
-      <c r="Y27" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="Z27">
-        <v>319</v>
-      </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB27" t="inlineStr">
-        <is>
-          <t>valmaggia_2014</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>CHR Population</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>CHR symptoms</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Van Tricht (2013)</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Van Tricht</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Carney (2017)</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>cannabis use</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Positive Symptoms</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>7.2999999999999995E-2</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>Hedges g</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>-0.536</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>0.681</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>0.815</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>VanTricht</t>
-        </is>
-      </c>
-      <c r="V28" t="inlineStr">
-        <is>
-          <t>CHR</t>
-        </is>
-      </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>vantricht_2013_chr</t>
-        </is>
-      </c>
-      <c r="X28" t="inlineStr">
-        <is>
-          <t>vantricht_2013</t>
-        </is>
-      </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>maybe</t>
-        </is>
-      </c>
-      <c r="Z28">
-        <v>322</v>
-      </c>
-      <c r="AA28" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB28" t="inlineStr">
-        <is>
-          <t>vantricht_2014</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>CHR Population</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>CHR symptoms</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Winton-Brown (2014)</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Winton-Brown</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Farris (2019)</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Cannabis use</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Negative Symptoms</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>Winton-Brown</t>
-        </is>
-      </c>
-      <c r="V29" t="inlineStr">
-        <is>
-          <t>CHR</t>
-        </is>
-      </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>winton-brown_2014_chr</t>
-        </is>
-      </c>
-      <c r="X29" t="inlineStr">
-        <is>
-          <t>winton-brown_2014</t>
-        </is>
-      </c>
-      <c r="Y29" t="inlineStr">
-        <is>
-          <t>maybe</t>
-        </is>
-      </c>
-      <c r="Z29">
-        <v>336</v>
-      </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB29" t="inlineStr">
-        <is>
-          <t>mustonen_2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Healthy Population</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Any psychosis outcome</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Zammit (2004)</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Zammit</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2004</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Moore (2007)</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>most frequent use</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Any psychosis outcome</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>longitudinal</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>1.72</t>
-        </is>
-      </c>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t>5.58</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>Zammit</t>
-        </is>
-      </c>
-      <c r="V30" t="inlineStr">
-        <is>
-          <t>HP</t>
-        </is>
-      </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>zammit_2004_hp</t>
-        </is>
-      </c>
-      <c r="X30" t="inlineStr">
-        <is>
-          <t>zammit_2004</t>
-        </is>
-      </c>
-      <c r="Y30" t="inlineStr">
-        <is>
-          <t>maybe</t>
-        </is>
-      </c>
-      <c r="Z30">
-        <v>339</v>
-      </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB30" t="inlineStr">
-        <is>
-          <t>zammit_2002</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Psychosis Population</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>relapse</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>van der Meer and Velthorst (2015)</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>van der Meer and Velthorst</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Schoeler (2016)</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>continued vs non-use</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Relapse</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>longitudinal</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>-0.08</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>Cohen's D</t>
-        </is>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>0·03</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>0·43</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>vanderMeerandVelthorst</t>
-        </is>
-      </c>
-      <c r="V31" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>vandermeerandvelthorst_2015_p</t>
-        </is>
-      </c>
-      <c r="X31" t="inlineStr">
-        <is>
-          <t>vandermeerandvelthorst_2015</t>
-        </is>
-      </c>
-      <c r="Y31" t="inlineStr">
-        <is>
-          <t>maybe</t>
-        </is>
-      </c>
-      <c r="Z31">
-        <v>315</v>
-      </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB31" t="inlineStr">
-        <is>
-          <t>vandermeer_2015</t>
+          <t>berger_2016</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
merge data with manually screened data info including reasons for exclusion
</commit_message>
<xml_diff>
--- a/02_data/cleandata/studies_to_check.xlsx
+++ b/02_data/cleandata/studies_to_check.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="Z2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="Z3">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
@@ -1112,22 +1112,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Kristensen and Cadenhead (2007)</t>
+          <t>Deighton (2016)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Kristensen and Cadenhead</t>
+          <t>Deighton</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>van der Meer (2012)</t>
+          <t>Oliver(2020)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1145,14 +1145,9 @@
           <t>cohort</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>KristensenandCadenhead</t>
+          <t>Deighton</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -1162,12 +1157,12 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>kristensenandcadenhead_2007_chr</t>
+          <t>deighton_2016_chr</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>kristensenandcadenhead_2007</t>
+          <t>deighton_2016</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -1176,7 +1171,7 @@
         </is>
       </c>
       <c r="Z8">
-        <v>171</v>
+        <v>76</v>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
@@ -1185,7 +1180,7 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>kristensen_2007</t>
+          <t>bechtold_2016</t>
         </is>
       </c>
     </row>
@@ -1202,17 +1197,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Bloeman (2010)</t>
+          <t>Lavoie (2014)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Bloemen</t>
+          <t>Lavoie</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1237,7 +1232,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>Bloemen</t>
+          <t>Lavoie</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
@@ -1247,12 +1242,12 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>bloemen_2010_chr</t>
+          <t>lavoie_2014_chr</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>bloemen_2010</t>
+          <t>lavoie_2014</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1261,7 +1256,7 @@
         </is>
       </c>
       <c r="Z9">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
@@ -1270,7 +1265,7 @@
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>bloemen_2009</t>
+          <t>lavoie_2012</t>
         </is>
       </c>
     </row>
@@ -1282,27 +1277,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>transition</t>
+          <t>CHR symptoms</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Deighton (2016)</t>
+          <t>Peters  (2009)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Deighton</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2009</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Oliver(2020)</t>
+          <t>Van de Meer(2012)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1312,7 +1307,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>transition to psychosis</t>
+          <t>CHR symptoms</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1320,9 +1315,14 @@
           <t>cohort</t>
         </is>
       </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>Deighton</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
@@ -1332,12 +1332,12 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>deighton_2016_chr</t>
+          <t>peters_2009_chr</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>deighton_2016</t>
+          <t>peters_2009</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -1346,7 +1346,7 @@
         </is>
       </c>
       <c r="Z10">
-        <v>76</v>
+        <v>231</v>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>bechtold_2016</t>
+          <t>patel_2019</t>
         </is>
       </c>
     </row>
@@ -1367,27 +1367,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>transition</t>
+          <t>CHR symptoms</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Lavoie (2014)</t>
+          <t>Van Tricht (2013)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Lavoie</t>
+          <t>Van Tricht</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Oliver(2020)</t>
+          <t>Carney (2017)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>transition to psychosis</t>
+          <t>Positive Symptoms</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1405,9 +1405,39 @@
           <t>cohort</t>
         </is>
       </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>7.2999999999999995E-2</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Hedges g</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>-0.536</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0.681</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>0.815</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>Lavoie</t>
+          <t>VanTricht</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
@@ -1417,12 +1447,12 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>lavoie_2014_chr</t>
+          <t>vantricht_2013_chr</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>lavoie_2014</t>
+          <t>vantricht_2013</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -1431,7 +1461,7 @@
         </is>
       </c>
       <c r="Z11">
-        <v>175</v>
+        <v>316</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
@@ -1440,7 +1470,7 @@
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>lavoie_2012</t>
+          <t>vantricht_2014</t>
         </is>
       </c>
     </row>
@@ -1457,32 +1487,32 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Peters  (2009)</t>
+          <t>Winton-Brown (2014)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Winton-Brown</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Van de Meer(2012)</t>
+          <t>Farris (2019)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>cannabis use</t>
+          <t>Cannabis use</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>CHR symptoms</t>
+          <t>Negative Symptoms</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1492,12 +1522,12 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Winton-Brown</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
@@ -1507,12 +1537,12 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>peters_2009_chr</t>
+          <t>winton-brown_2014_chr</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>peters_2009</t>
+          <t>winton-brown_2014</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -1521,7 +1551,7 @@
         </is>
       </c>
       <c r="Z12">
-        <v>232</v>
+        <v>330</v>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
@@ -1530,7 +1560,7 @@
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>patel_2019</t>
+          <t>mustonen_2018</t>
         </is>
       </c>
     </row>
@@ -1542,22 +1572,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CHR symptoms</t>
+          <t>CHR state</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Van Tricht (2013)</t>
+          <t>Addington (2012)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Van Tricht</t>
+          <t>Addington</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1567,12 +1597,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>cannabis use</t>
+          <t>current cannabis use</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Positive Symptoms</t>
+          <t>CHR state</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1582,37 +1612,37 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>7.2999999999999995E-2</t>
+          <t>1.556</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Hedges g</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>-0.536</t>
+          <t>1.061</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>0.681</t>
+          <t>2.28</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>0.023</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>VanTricht</t>
+          <t>Addington</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
@@ -1622,12 +1652,12 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>vantricht_2013_chr</t>
+          <t>addington_2012_chr</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>vantricht_2013</t>
+          <t>addington_2012</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
@@ -1636,7 +1666,7 @@
         </is>
       </c>
       <c r="Z13">
-        <v>317</v>
+        <v>4</v>
       </c>
       <c r="AA13" t="inlineStr">
         <is>
@@ -1645,79 +1675,99 @@
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>vantricht_2014</t>
+          <t>addington_2017</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CHR Population</t>
+          <t>Psychosis Population</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CHR symptoms</t>
+          <t>symptoms</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Winton-Brown (2014)</t>
+          <t>Degenhardt (2007)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Winton-Brown</t>
+          <t>Degenhardt</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Farris (2019)</t>
+          <t>Zammit (2008)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Cannabis use</t>
+          <t>cannabis use</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Negative Symptoms</t>
+          <t>positive symptoms</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>cohort</t>
+          <t>longitudinal</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>0.26</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>Winton-Brown</t>
+          <t>Degenhardt</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>CHR</t>
+          <t>P</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>winton-brown_2014_chr</t>
+          <t>degenhardt_2007_p</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>winton-brown_2014</t>
+          <t>degenhardt_2007</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
@@ -1726,7 +1776,7 @@
         </is>
       </c>
       <c r="Z14">
-        <v>331</v>
+        <v>73</v>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
@@ -1735,104 +1785,84 @@
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>mustonen_2018</t>
+          <t>degenhardt_2001</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CHR Population</t>
+          <t>Psychosis Population</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CHR state</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Addington (2012)</t>
+          <t>Hadden (2016)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Addington</t>
+          <t>Hadden</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Carney (2017)</t>
+          <t>Athanassiou (2021)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>current cannabis use</t>
+          <t>cannabis use</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>CHR state</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>cohort</t>
+          <t>longitudinal</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>1.556</t>
+          <t>-0.1</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>1.061</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>2.28</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>0.023</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>Yes</t>
+          <t>B estimate</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>Addington</t>
+          <t>Hadden</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>CHR</t>
+          <t>P</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>addington_2012_chr</t>
+          <t>hadden_2016_p</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>addington_2012</t>
+          <t>hadden_2018</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -1841,7 +1871,7 @@
         </is>
       </c>
       <c r="Z15">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
@@ -1850,7 +1880,7 @@
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>addington_2017</t>
+          <t>hadden_2026</t>
         </is>
       </c>
     </row>
@@ -1862,27 +1892,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>symptoms</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Degenhardt (2007)</t>
+          <t>Seddon (2016)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Degenhardt</t>
+          <t>Seddon</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Zammit (2008)</t>
+          <t>Athanassiou (2021)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1892,7 +1922,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>positive symptoms</t>
+          <t>any psychosis outcome</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1902,32 +1932,17 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>2.14</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>0.26</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>Yes</t>
+          <t>B estimate</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>Degenhardt</t>
+          <t>Seddon</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
@@ -1937,12 +1952,12 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>degenhardt_2007_p</t>
+          <t>seddon_2016_p</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>degenhardt_2007</t>
+          <t>seddon_2016</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
@@ -1951,7 +1966,7 @@
         </is>
       </c>
       <c r="Z16">
-        <v>73</v>
+        <v>276</v>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
@@ -1960,7 +1975,7 @@
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>degenhardt_2001</t>
+          <t>seddon_2015</t>
         </is>
       </c>
     </row>
@@ -1977,17 +1992,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Hadden (2016)</t>
+          <t>Bhattacharrya (2020)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Hadden</t>
+          <t>Bhattacharrya</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2012,17 +2027,17 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>-0.1</t>
+          <t>3.44</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>B estimate</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>Hadden</t>
+          <t>Bhattacharrya</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
@@ -2032,12 +2047,12 @@
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>hadden_2016_p</t>
+          <t>bhattacharrya_2020_p</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>hadden_2018</t>
+          <t>bhattacharrya_2020</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -2046,7 +2061,7 @@
         </is>
       </c>
       <c r="Z17">
-        <v>133</v>
+        <v>38</v>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
@@ -2055,84 +2070,89 @@
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>hadden_2026</t>
+          <t>harley_2010</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>Environmental Moderators</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Bechtold (2015)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Bechtold</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Hosseini(2019)</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Age of first use</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>any psychosis outcome</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Oullette-Plamondon (2017)</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Ouellett-Plamondon</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Athanassiou (2021)</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>cannabis use</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>any psychosis outcome</t>
-        </is>
-      </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>longitudinal</t>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>506</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0.9</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>Cohen's D</t>
+          <t>in tabelle (supplementary material, Appendix 3)</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>Ouellett-Plamondon</t>
+          <t>Bechtold</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>EnvMod</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>ouellett-plamondon_2017_p</t>
+          <t>bechtold_2015_envmod</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>ouellett-plamondon_2017</t>
+          <t>bechtold_2015</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -2141,7 +2161,7 @@
         </is>
       </c>
       <c r="Z18">
-        <v>224</v>
+        <v>33</v>
       </c>
       <c r="AA18" t="inlineStr">
         <is>
@@ -2150,84 +2170,89 @@
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>ouellet-plamondon_2017</t>
+          <t>bechtold_2016</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>Environmental Moderators</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Henquet (2004)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Henquet</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Hosseini(2019)</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Age of first use</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
           <t>any psychosis outcome</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Seddon (2016)</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Seddon</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Athanassiou (2021)</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>cannabis use</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>any psychosis outcome</t>
-        </is>
-      </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>longitudinal</t>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2437</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2.14</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>B estimate</t>
+          <t>in tabelle (supplementary material, Appendix 3)</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>Seddon</t>
+          <t>Henquet</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>EnvMod</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>seddon_2016_p</t>
+          <t>henquet_2004_envmod</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>seddon_2016</t>
+          <t>henquet_2004</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -2236,7 +2261,7 @@
         </is>
       </c>
       <c r="Z19">
-        <v>277</v>
+        <v>138</v>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
@@ -2245,84 +2270,89 @@
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>seddon_2015</t>
+          <t>henquet_2005</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Psychosis Population</t>
+          <t>Environmental Moderators</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>Environmental Moderators</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Di Forti (2014)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Di Forti</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Hosseini(2019)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Age of first use</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
           <t>any psychosis outcome</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Bhattacharrya (2020)</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Bhattacharrya</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Athanassiou (2021)</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>cannabis use</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>any psychosis outcome</t>
-        </is>
-      </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>longitudinal</t>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>410</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>3.44</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>OR</t>
+          <t>in tabelle (supplementary material, Appendix 3)</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>Bhattacharrya</t>
+          <t>DiForti</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>EnvMod</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>bhattacharrya_2020_p</t>
+          <t>diforti_2014_envmod</t>
         </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>bhattacharrya_2020</t>
+          <t>diforti_2014</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
@@ -2331,7 +2361,7 @@
         </is>
       </c>
       <c r="Z20">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
@@ -2340,7 +2370,7 @@
       </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>harley_2010</t>
+          <t>diforti_2009</t>
         </is>
       </c>
     </row>
@@ -2357,27 +2387,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Bechtold (2015)</t>
+          <t>Marwaha (2018)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Bechtold</t>
+          <t>Marwaha</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Hosseini(2019)</t>
+          <t>Godin(2022)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Age of first use</t>
+          <t>High cannabis use</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -2387,27 +2417,17 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>506</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>in tabelle (supplementary material, Appendix 3)</t>
+          <t>longitudinal</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>Bechtold</t>
+          <t>Marwaha</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
@@ -2417,12 +2437,12 @@
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>bechtold_2015_envmod</t>
+          <t>marwaha_2018_envmod</t>
         </is>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>bechtold_2015</t>
+          <t>marwaha_2018</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2431,7 +2451,7 @@
         </is>
       </c>
       <c r="Z21">
-        <v>33</v>
+        <v>194</v>
       </c>
       <c r="AA21" t="inlineStr">
         <is>
@@ -2440,7 +2460,7 @@
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>bechtold_2016</t>
+          <t>mizrahi_2014</t>
         </is>
       </c>
     </row>
@@ -2457,27 +2477,27 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Henquet (2004)</t>
+          <t>Albertella (2018)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Henquet</t>
+          <t>Albertella</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Hosseini(2019)</t>
+          <t>Polkosnik(2021)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Age of first use</t>
+          <t>Low cannabis use</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -2487,17 +2507,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>2437</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>in tabelle (supplementary material, Appendix 3)</t>
+          <t>prospective cohort</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2507,7 +2517,7 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>Henquet</t>
+          <t>Albertella</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
@@ -2517,21 +2527,21 @@
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>henquet_2004_envmod</t>
+          <t>albertella_2018_envmod</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>henquet_2004</t>
+          <t>albertella_2018</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>maybe</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="Z22">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="AA22" t="inlineStr">
         <is>
@@ -2539,286 +2549,6 @@
         </is>
       </c>
       <c r="AB22" t="inlineStr">
-        <is>
-          <t>henquet_2005</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Environmental Moderators</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Environmental Moderators</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Di Forti (2014)</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Di Forti</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Hosseini(2019)</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Age of first use</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>any psychosis outcome</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>cohort</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>410</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>in tabelle (supplementary material, Appendix 3)</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>DiForti</t>
-        </is>
-      </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>EnvMod</t>
-        </is>
-      </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>diforti_2014_envmod</t>
-        </is>
-      </c>
-      <c r="X23" t="inlineStr">
-        <is>
-          <t>diforti_2014</t>
-        </is>
-      </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>maybe</t>
-        </is>
-      </c>
-      <c r="Z23">
-        <v>86</v>
-      </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB23" t="inlineStr">
-        <is>
-          <t>diforti_2009</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Environmental Moderators</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Environmental Moderators</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Marwaha (2018)</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Marwaha</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Godin(2022)</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>High cannabis use</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>any psychosis outcome</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>longitudinal</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>Marwaha</t>
-        </is>
-      </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>EnvMod</t>
-        </is>
-      </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>marwaha_2018_envmod</t>
-        </is>
-      </c>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>marwaha_2018</t>
-        </is>
-      </c>
-      <c r="Y24" t="inlineStr">
-        <is>
-          <t>maybe</t>
-        </is>
-      </c>
-      <c r="Z24">
-        <v>195</v>
-      </c>
-      <c r="AA24" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB24" t="inlineStr">
-        <is>
-          <t>mizrahi_2014</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Environmental Moderators</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Environmental Moderators</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Albertella (2018)</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Albertella</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Polkosnik(2021)</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Low cannabis use</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>any psychosis outcome</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>prospective cohort</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>Albertella</t>
-        </is>
-      </c>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>EnvMod</t>
-        </is>
-      </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>albertella_2018_envmod</t>
-        </is>
-      </c>
-      <c r="X25" t="inlineStr">
-        <is>
-          <t>albertella_2018</t>
-        </is>
-      </c>
-      <c r="Y25" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="Z25">
-        <v>8</v>
-      </c>
-      <c r="AA25" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB25" t="inlineStr">
         <is>
           <t>berger_2016</t>
         </is>

</xml_diff>